<commit_message>
Descrição das mudanças feitas após o stash
</commit_message>
<xml_diff>
--- a/core/utils/cadastrodeitens.xlsx
+++ b/core/utils/cadastrodeitens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ventura System\Ventura Back-End\project-beck_ventura\core\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037CFE2A-DC8D-4EFA-9A0F-FEB6C6ADE140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A80EDFA-629E-4918-AB48-D59BBC4E13ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9029D061-8B28-4E8B-B87C-E01B1A6C0E7F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>PROJETO</t>
   </si>
@@ -105,34 +105,22 @@
     <t>00</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>EG/LG</t>
   </si>
   <si>
-    <t>camiseta manga curta</t>
+    <t>SANTO ANDRÉ</t>
   </si>
   <si>
-    <t>unissex</t>
+    <t>KIT VERÃO</t>
   </si>
   <si>
-    <t>cubatão</t>
+    <t>UNISSEX</t>
   </si>
   <si>
-    <t>masculino</t>
+    <t>KIT INVERNO</t>
   </si>
   <si>
-    <t>feminino</t>
-  </si>
-  <si>
-    <t>camiseta regata</t>
-  </si>
-  <si>
-    <t>bermuda</t>
-  </si>
-  <si>
-    <t>camiseta manga longa</t>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -743,7 +731,7 @@
   <dimension ref="A1:AA784"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -830,7 +818,7 @@
         <v>14</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>20</v>
@@ -838,64 +826,62 @@
     </row>
     <row r="2" spans="1:27" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="T2" s="20"/>
       <c r="U2" s="21" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="V2" s="21"/>
-      <c r="W2" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="W2" s="21"/>
       <c r="X2" s="21"/>
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
@@ -903,324 +889,178 @@
     </row>
     <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="T3" s="20"/>
       <c r="U3" s="21" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="V3" s="21"/>
-      <c r="W3" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="W3" s="21"/>
       <c r="X3" s="21"/>
       <c r="Y3" s="21"/>
       <c r="Z3" s="21"/>
       <c r="AA3" s="21"/>
     </row>
     <row r="4" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
       <c r="O4" s="20"/>
-      <c r="P4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
       <c r="T4" s="20"/>
-      <c r="U4" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="U4" s="21"/>
       <c r="V4" s="21"/>
-      <c r="W4" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="W4" s="21"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
       <c r="O5" s="20"/>
-      <c r="P5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
       <c r="T5" s="20"/>
-      <c r="U5" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="U5" s="21"/>
       <c r="V5" s="21"/>
-      <c r="W5" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="W5" s="21"/>
       <c r="X5" s="21"/>
       <c r="Y5" s="21"/>
       <c r="Z5" s="21"/>
       <c r="AA5" s="21"/>
     </row>
     <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
-      <c r="F6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
       <c r="O6" s="20"/>
-      <c r="P6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
       <c r="T6" s="20"/>
-      <c r="U6" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="U6" s="21"/>
       <c r="V6" s="21"/>
-      <c r="W6" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="W6" s="21"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="21"/>
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="R7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="S7" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
       <c r="T7" s="20"/>
-      <c r="U7" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="U7" s="21"/>
       <c r="V7" s="21"/>
-      <c r="W7" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="W7" s="21"/>
       <c r="X7" s="21"/>
       <c r="Y7" s="21"/>
       <c r="Z7" s="21"/>

</xml_diff>